<commit_message>
added interview consent form
</commit_message>
<xml_diff>
--- a/docs/Getana_Deliverable_1_DailyScrumReport.xlsx
+++ b/docs/Getana_Deliverable_1_DailyScrumReport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
   <si>
     <t xml:space="preserve">Daily Scrum Report</t>
   </si>
@@ -101,6 +101,45 @@
   </si>
   <si>
     <t xml:space="preserve">10 Feb 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: Absent from meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What impediments prevent them from progressing: None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: Installed Android Studio, Reqs and Use Cases for stories 4-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they will do: interview scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What impediments prevent them from progressing: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: Installed Android Studio, user reqs for 1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they will do: system reqs and use cases for 1-3, mockup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: reqs and use cases for stories 13-15, created various documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they will do: Permission form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they have done: Installed Android Studio, reqs for 10-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What they will do: reqs for 19, use cases for 10-19 and 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx Feb 18</t>
   </si>
 </sst>
 </file>
@@ -267,10 +306,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +534,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,12 +542,12 @@
         <v>14</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,7 +560,7 @@
         <v>17</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,7 +570,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,17 +578,17 @@
         <v>19</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,17 +596,17 @@
         <v>21</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,16 +614,146 @@
         <v>23</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="0" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created unified requirements doc
</commit_message>
<xml_diff>
--- a/docs/Getana_Deliverable_1_DailyScrumReport.xlsx
+++ b/docs/Getana_Deliverable_1_DailyScrumReport.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">What they have done: Nothing</t>
   </si>
   <si>
-    <t xml:space="preserve">What they will do: Install ZenHub. Install UMLet. Install Android Studio.</t>
+    <t xml:space="preserve">What will they do: Learn how to do use cases, install UMLet, install Android Studio, install ZenHub</t>
   </si>
   <si>
     <t xml:space="preserve">What impediments prevent them from progressing: </t>
@@ -311,8 +311,8 @@
   </sheetPr>
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>